<commit_message>
fix variable (the problem with Jupyter notebooks)
</commit_message>
<xml_diff>
--- a/output/fRAT_new__check_2,3_solution_True.xlsx
+++ b/output/fRAT_new__check_2,3_solution_True.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rejna\Work_only_here\Miscellaneous\rakshitha\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rejna\Work_only_here\Miscellaneous\rakshitha\r_m_thesis\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F918919-8711-4622-8D58-A7A37DB718E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EAFCDF-5F58-4AF3-9BC3-6D866D58176C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1179,11 +1179,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="30.08984375" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>